<commit_message>
run(Excel): Run CSV pyrhon script on Eolian Fenix file
</commit_message>
<xml_diff>
--- a/StressXbeeResults.xlsx
+++ b/StressXbeeResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ma\Documents\Github\Telemetria_Auriga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1074D6CD-C885-4088-99AB-13270373C750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3B493A-E8AB-435B-A5F3-3DC016D94FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{ADC039E0-CD57-44FC-82F1-8A513F14123F}"/>
+    <workbookView xWindow="-60" yWindow="16080" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{ADC039E0-CD57-44FC-82F1-8A513F14123F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Bitrate</t>
   </si>
@@ -59,13 +59,16 @@
   <si>
     <t>Tamaño mensaje [Bytes]</t>
   </si>
+  <si>
+    <t>Throughput (bps)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -110,9 +113,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -133,6 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
@@ -12705,7 +12709,7 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I115"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13651,7 +13655,7 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15956,8 +15960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B6FF5E-A242-4066-BF7B-FF822A4A3704}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J116" sqref="J116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19725,12 +19729,15 @@
         <f t="shared" si="0"/>
         <v>5009.4476424836303</v>
       </c>
-      <c r="J120">
-        <f t="shared" si="0"/>
+      <c r="J120" s="8">
+        <f>MAX(J3:J116)</f>
         <v>7212.90730781398</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
       <c r="B121">
         <f>B120*8</f>
         <v>787.33903578594004</v>
@@ -19764,7 +19771,7 @@
         <v>40075.581139869042</v>
       </c>
       <c r="J121">
-        <f t="shared" si="1"/>
+        <f>J120*8</f>
         <v>57703.25846251184</v>
       </c>
     </row>

</xml_diff>